<commit_message>
<Test case, defects and execution report>
</commit_message>
<xml_diff>
--- a/Testcases/Testcase Sheet.xlsx
+++ b/Testcases/Testcase Sheet.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
     <sheet name="Test cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Defects" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Test cases are in Test cases tab of this sheet</t>
   </si>
@@ -136,6 +137,45 @@
   </si>
   <si>
     <t>Error message should appear on clicking Submit button as "Invalid email format. Please enter format as Ex. name@example.com"</t>
+  </si>
+  <si>
+    <t>Defect Description</t>
+  </si>
+  <si>
+    <t>Defect Steps</t>
+  </si>
+  <si>
+    <t>Actual condition</t>
+  </si>
+  <si>
+    <t>December month page shows blank page</t>
+  </si>
+  <si>
+    <t>1. Open rb shoe site
+2. Click December month link
+3. Verify that if no shoe present it should show Coming Soon text</t>
+  </si>
+  <si>
+    <t>December page shows blank without any message</t>
+  </si>
+  <si>
+    <t>November month page does not show shoe image</t>
+  </si>
+  <si>
+    <t>1. Open rb shoe site
+2. Click November month link
+3. Verify that page should show image of shoe</t>
+  </si>
+  <si>
+    <t>Month page: Description tag alignment not proper</t>
+  </si>
+  <si>
+    <t>1. Open rb shoe site
+2. Open any month page
+3. Verify Description tag alignment</t>
+  </si>
+  <si>
+    <t>Description tag alignment is not proper</t>
   </si>
 </sst>
 </file>
@@ -569,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -728,4 +768,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>